<commit_message>
Updated code for excel utility
</commit_message>
<xml_diff>
--- a/externalFiles/playwright.xlsx
+++ b/externalFiles/playwright.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>srno</t>
   </si>
@@ -22,7 +22,7 @@
     <t>age</t>
   </si>
   <si>
-    <t>NoWow100</t>
+    <t>NoWow900</t>
   </si>
   <si>
     <t>city</t>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>nagpur</t>
-  </si>
-  <si>
-    <t>maharashtra</t>
   </si>
 </sst>
 </file>
@@ -344,8 +341,8 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
+      <c r="F2" s="1">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>